<commit_message>
fixed excels mango burkina and milk burundi
</commit_message>
<xml_diff>
--- a/data/xls/eco/IKMS Tranfer AFA Burundi Lait.xlsx
+++ b/data/xls/eco/IKMS Tranfer AFA Burundi Lait.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="127">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -342,9 +342,6 @@
     <t xml:space="preserve">Receiver Name</t>
   </si>
   <si>
-    <t xml:space="preserve">value (local currency)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Land owners (land fees)</t>
   </si>
   <si>
@@ -354,7 +351,7 @@
     <t xml:space="preserve">Employees (wages)</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial institutions (interests On loans)</t>
+    <t xml:space="preserve">Financial institutions (interests on loans)</t>
   </si>
   <si>
     <t xml:space="preserve">Government (taxes - subsidies)</t>
@@ -568,7 +565,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.33"/>
@@ -590,37 +587,37 @@
         <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>2</v>
@@ -634,37 +631,37 @@
         <v>767135.966288091</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>221289.221044642</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,37 +672,37 @@
         <v>752885.310891548</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>217178.45506487</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,37 +713,37 @@
         <v>347670.319149328</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>36215.6573452961</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>19315.0172508246</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>1241.67968041015</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>1448.62629381185</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,37 +754,37 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,37 +795,37 @@
         <v>7480.60000943869</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>77683.1507287011</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,37 +836,37 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>474752.445504823</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,37 +877,37 @@
         <v>11965.0222586716</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,37 +918,37 @@
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>607298.251305831</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,37 +959,37 @@
         <v>117734.640866035</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>90565.1061092797</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,37 +1000,37 @@
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>39290.0395350325</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>7619.8864036676</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>1959.3993609431</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>1714.47448340464</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,37 +1041,37 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>21654.9243282192</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>5774.64648752512</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>3341.04532948945</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>433.098486564384</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,37 +1082,37 @@
         <v>1806989.5428543</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>521246.983515662</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1137,7 @@
       <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
@@ -1157,10 +1154,10 @@
         <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -1174,10 +1171,10 @@
         <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>2750.84413101868</v>
@@ -1191,10 +1188,10 @@
         <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>4439.83919241145</v>
@@ -1208,10 +1205,10 @@
         <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>13654.4841178922</v>
@@ -1225,10 +1222,10 @@
         <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>2983.31386141011</v>
@@ -1242,10 +1239,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>120.946766520263</v>
@@ -1259,10 +1256,10 @@
         <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>865.896116481989</v>
@@ -1276,10 +1273,10 @@
         <v>52</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>13.6872472670178</v>
@@ -1293,10 +1290,10 @@
         <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>
@@ -1310,10 +1307,10 @@
         <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1327,10 +1324,10 @@
         <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>41.0541755671076</v>
@@ -1344,10 +1341,10 @@
         <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>17.953433093075</v>
@@ -1361,10 +1358,10 @@
         <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>0</v>
@@ -1378,10 +1375,10 @@
         <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
@@ -1395,10 +1392,10 @@
         <v>61</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>0</v>
@@ -1412,10 +1409,10 @@
         <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -1429,10 +1426,10 @@
         <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -1446,10 +1443,10 @@
         <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>2105.43113264954</v>
@@ -1463,10 +1460,10 @@
         <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>9457.71348197013</v>
@@ -1480,10 +1477,10 @@
         <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>14369.654798043</v>
@@ -1497,10 +1494,10 @@
         <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>17025.5780433751</v>
@@ -1514,10 +1511,10 @@
         <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>14102.9557483952</v>
@@ -1531,10 +1528,10 @@
         <v>51</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>4758.96534664921</v>
@@ -1548,10 +1545,10 @@
         <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>1708.75554927543</v>
@@ -1565,10 +1562,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>38588.1539915245</v>
@@ -1582,10 +1579,10 @@
         <v>54</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>11924.3229524614</v>
@@ -1599,10 +1596,10 @@
         <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>13715.7333486924</v>
@@ -1616,10 +1613,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>1330.79847025831</v>
@@ -1633,10 +1630,10 @@
         <v>58</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>24677.4267620632</v>
@@ -1650,10 +1647,10 @@
         <v>60</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -1667,10 +1664,10 @@
         <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>0</v>
@@ -1684,10 +1681,10 @@
         <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>0</v>
@@ -1701,10 +1698,10 @@
         <v>63</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0</v>
@@ -1718,10 +1715,10 @@
         <v>46</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -1735,10 +1732,10 @@
         <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -1752,10 +1749,10 @@
         <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -1769,10 +1766,10 @@
         <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -1786,10 +1783,10 @@
         <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
@@ -1803,10 +1800,10 @@
         <v>51</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>58.4479914299166</v>
@@ -1820,10 +1817,10 @@
         <v>52</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
@@ -1837,10 +1834,10 @@
         <v>53</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
@@ -1854,10 +1851,10 @@
         <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>0</v>
@@ -1871,10 +1868,10 @@
         <v>56</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>0</v>
@@ -1888,10 +1885,10 @@
         <v>57</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>0</v>
@@ -1905,10 +1902,10 @@
         <v>58</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>0</v>
@@ -1922,10 +1919,10 @@
         <v>60</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>0</v>
@@ -1939,10 +1936,10 @@
         <v>61</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>0</v>
@@ -1956,10 +1953,10 @@
         <v>62</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" s="2" t="n">
         <v>0</v>
@@ -1973,10 +1970,10 @@
         <v>63</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>0</v>
@@ -1990,10 +1987,10 @@
         <v>46</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
@@ -2007,10 +2004,10 @@
         <v>47</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E51" s="2" t="n">
         <v>0</v>
@@ -2024,10 +2021,10 @@
         <v>48</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E52" s="2" t="n">
         <v>0</v>
@@ -2041,10 +2038,10 @@
         <v>49</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>0</v>
@@ -2058,10 +2055,10 @@
         <v>50</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E54" s="2" t="n">
         <v>0</v>
@@ -2075,10 +2072,10 @@
         <v>51</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>0</v>
@@ -2092,10 +2089,10 @@
         <v>52</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56" s="2" t="n">
         <v>0</v>
@@ -2109,10 +2106,10 @@
         <v>53</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E57" s="2" t="n">
         <v>0</v>
@@ -2126,10 +2123,10 @@
         <v>54</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E58" s="2" t="n">
         <v>0</v>
@@ -2143,10 +2140,10 @@
         <v>56</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E59" s="2" t="n">
         <v>149.113248908792</v>
@@ -2160,10 +2157,10 @@
         <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E60" s="2" t="n">
         <v>112.208998469536</v>
@@ -2177,10 +2174,10 @@
         <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E61" s="2" t="n">
         <v>0</v>
@@ -2194,10 +2191,10 @@
         <v>60</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E62" s="2" t="n">
         <v>0</v>
@@ -2211,10 +2208,10 @@
         <v>61</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E63" s="2" t="n">
         <v>0</v>
@@ -2228,10 +2225,10 @@
         <v>62</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E64" s="2" t="n">
         <v>0</v>
@@ -2245,10 +2242,10 @@
         <v>63</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E65" s="2" t="n">
         <v>0</v>
@@ -2262,10 +2259,10 @@
         <v>46</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E66" s="2" t="n">
         <v>7136.6790744488</v>
@@ -2279,10 +2276,10 @@
         <v>47</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E67" s="2" t="n">
         <v>6223.0362003648</v>
@@ -2296,10 +2293,10 @@
         <v>48</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E68" s="2" t="n">
         <v>17444.1461494702</v>
@@ -2313,10 +2310,10 @@
         <v>49</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>10941.9222699632</v>
@@ -2330,10 +2327,10 @@
         <v>50</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E70" s="2" t="n">
         <v>81.752117035302</v>
@@ -2347,10 +2344,10 @@
         <v>51</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E71" s="2" t="n">
         <v>76.2396890811469</v>
@@ -2364,10 +2361,10 @@
         <v>52</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>734.464823495301</v>
@@ -2381,10 +2378,10 @@
         <v>53</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E73" s="2" t="n">
         <v>5667.63292753216</v>
@@ -2398,10 +2395,10 @@
         <v>54</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E74" s="2" t="n">
         <v>1173.86239343195</v>
@@ -2415,10 +2412,10 @@
         <v>56</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>724.285703542013</v>
@@ -2432,10 +2429,10 @@
         <v>57</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E76" s="2" t="n">
         <v>177.290225027688</v>
@@ -2449,10 +2446,10 @@
         <v>58</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E77" s="2" t="n">
         <v>9232.43687834594</v>
@@ -2466,10 +2463,10 @@
         <v>60</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E78" s="2" t="n">
         <v>0</v>
@@ -2483,10 +2480,10 @@
         <v>61</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E79" s="2" t="n">
         <v>0</v>
@@ -2500,10 +2497,10 @@
         <v>62</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E80" s="2" t="n">
         <v>0</v>
@@ -2517,10 +2514,10 @@
         <v>63</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E81" s="2" t="n">
         <v>0</v>
@@ -2534,10 +2531,10 @@
         <v>46</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E82" s="2" t="n">
         <v>13645.028477021</v>
@@ -2551,10 +2548,10 @@
         <v>47</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E83" s="2" t="n">
         <v>21453.0795799329</v>
@@ -2568,10 +2565,10 @@
         <v>48</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E84" s="2" t="n">
         <v>46800.4747732908</v>
@@ -2585,10 +2582,10 @@
         <v>49</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E85" s="2" t="n">
         <v>34055.7864722794</v>
@@ -2602,10 +2599,10 @@
         <v>50</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E86" s="2" t="n">
         <v>15153.1829911701</v>
@@ -2619,10 +2616,10 @@
         <v>51</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E87" s="2" t="n">
         <v>7272.48900066694</v>
@@ -2636,10 +2633,10 @@
         <v>52</v>
       </c>
       <c r="C88" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D88" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E88" s="2" t="n">
         <v>3098.43191764212</v>
@@ -2653,10 +2650,10 @@
         <v>53</v>
       </c>
       <c r="C89" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E89" s="2" t="n">
         <v>44255.7869190567</v>
@@ -2670,10 +2667,10 @@
         <v>54</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E90" s="2" t="n">
         <v>14213.137423961</v>
@@ -2687,10 +2684,10 @@
         <v>56</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E91" s="2" t="n">
         <v>14958.5237710325</v>
@@ -2704,10 +2701,10 @@
         <v>57</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E92" s="2" t="n">
         <v>1750.46012531815</v>
@@ -2721,10 +2718,10 @@
         <v>58</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E93" s="2" t="n">
         <v>36290.0825107558</v>
@@ -2738,10 +2735,10 @@
         <v>60</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E94" s="2" t="n">
         <v>0</v>
@@ -2755,10 +2752,10 @@
         <v>61</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E95" s="2" t="n">
         <v>0</v>
@@ -2772,10 +2769,10 @@
         <v>62</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E96" s="2" t="n">
         <v>0</v>
@@ -2789,10 +2786,10 @@
         <v>63</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E97" s="2" t="n">
         <v>0</v>
@@ -2806,10 +2803,10 @@
         <v>46</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E98" s="2" t="n">
         <v>26.4823468169197</v>
@@ -2823,10 +2820,10 @@
         <v>47</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E99" s="2" t="n">
         <v>421.571727842093</v>
@@ -2840,10 +2837,10 @@
         <v>48</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E100" s="2" t="n">
         <v>2615.48118178577</v>
@@ -2857,10 +2854,10 @@
         <v>49</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E101" s="2" t="n">
         <v>224.312439614243</v>
@@ -2874,10 +2871,10 @@
         <v>50</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E102" s="2" t="n">
         <v>129.884424696022</v>
@@ -2891,10 +2888,10 @@
         <v>51</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E103" s="2" t="n">
         <v>0</v>
@@ -2908,10 +2905,10 @@
         <v>52</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E104" s="2" t="n">
         <v>0</v>
@@ -2925,10 +2922,10 @@
         <v>53</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E105" s="2" t="n">
         <v>0</v>
@@ -2942,10 +2939,10 @@
         <v>54</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E106" s="2" t="n">
         <v>0</v>
@@ -2959,10 +2956,10 @@
         <v>56</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E107" s="2" t="n">
         <v>0</v>
@@ -2976,10 +2973,10 @@
         <v>57</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E108" s="2" t="n">
         <v>0</v>
@@ -2993,10 +2990,10 @@
         <v>58</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E109" s="2" t="n">
         <v>0</v>
@@ -3010,10 +3007,10 @@
         <v>60</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E110" s="2" t="n">
         <v>0</v>
@@ -3027,10 +3024,10 @@
         <v>61</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E111" s="2" t="n">
         <v>0</v>
@@ -3044,10 +3041,10 @@
         <v>62</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E112" s="2" t="n">
         <v>0</v>
@@ -3061,10 +3058,10 @@
         <v>63</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E113" s="2" t="n">
         <v>0</v>
@@ -3078,10 +3075,10 @@
         <v>46</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E114" s="2" t="n">
         <v>0</v>
@@ -3095,10 +3092,10 @@
         <v>47</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E115" s="2" t="n">
         <v>0</v>
@@ -3112,10 +3109,10 @@
         <v>48</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E116" s="2" t="n">
         <v>0</v>
@@ -3129,10 +3126,10 @@
         <v>49</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E117" s="2" t="n">
         <v>0</v>
@@ -3146,10 +3143,10 @@
         <v>50</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E118" s="2" t="n">
         <v>108.237020580018</v>
@@ -3163,10 +3160,10 @@
         <v>51</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E119" s="2" t="n">
         <v>60.6820051322966</v>
@@ -3180,10 +3177,10 @@
         <v>52</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E120" s="2" t="n">
         <v>0</v>
@@ -3197,10 +3194,10 @@
         <v>53</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E121" s="2" t="n">
         <v>0</v>
@@ -3214,10 +3211,10 @@
         <v>54</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E122" s="2" t="n">
         <v>0.923016012405848</v>
@@ -3231,10 +3228,10 @@
         <v>56</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E123" s="2" t="n">
         <v>3.31362839002792</v>
@@ -3248,10 +3245,10 @@
         <v>57</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E124" s="2" t="n">
         <v>0</v>
@@ -3265,10 +3262,10 @@
         <v>58</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E125" s="2" t="n">
         <v>101.407131923486</v>
@@ -3282,10 +3279,10 @@
         <v>60</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E126" s="2" t="n">
         <v>0</v>
@@ -3299,10 +3296,10 @@
         <v>61</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E127" s="2" t="n">
         <v>0</v>
@@ -3316,10 +3313,10 @@
         <v>62</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E128" s="2" t="n">
         <v>0</v>
@@ -3333,10 +3330,10 @@
         <v>63</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E129" s="2" t="n">
         <v>0</v>
@@ -3350,10 +3347,10 @@
         <v>46</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E130" s="2" t="n">
         <v>1438.37991535664</v>
@@ -3367,10 +3364,10 @@
         <v>47</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E131" s="2" t="n">
         <v>1411.65993688628</v>
@@ -3384,10 +3381,10 @@
         <v>48</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E132" s="2" t="n">
         <v>3388.1053423651</v>
@@ -3401,10 +3398,10 @@
         <v>49</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E133" s="2" t="n">
         <v>2915.03160626799</v>
@@ -3418,10 +3415,10 @@
         <v>50</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E134" s="2" t="n">
         <v>869.175763335379</v>
@@ -3435,10 +3432,10 @@
         <v>51</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E135" s="2" t="n">
         <v>342.89488305551</v>
@@ -3452,10 +3449,10 @@
         <v>52</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E136" s="2" t="n">
         <v>259.859088066428</v>
@@ -3469,10 +3466,10 @@
         <v>53</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E137" s="2" t="n">
         <v>0</v>
@@ -3486,10 +3483,10 @@
         <v>54</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E138" s="2" t="n">
         <v>17.9475333880074</v>
@@ -3503,10 +3500,10 @@
         <v>56</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E139" s="2" t="n">
         <v>294.336590469202</v>
@@ -3520,10 +3517,10 @@
         <v>57</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E140" s="2" t="n">
         <v>112.208998469536</v>
@@ -3537,10 +3534,10 @@
         <v>58</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E141" s="2" t="n">
         <v>2278.81173842315</v>
@@ -3554,10 +3551,10 @@
         <v>60</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E142" s="2" t="n">
         <v>0</v>
@@ -3571,10 +3568,10 @@
         <v>61</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E143" s="2" t="n">
         <v>0</v>
@@ -3588,10 +3585,10 @@
         <v>62</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E144" s="2" t="n">
         <v>0</v>
@@ -3605,10 +3602,10 @@
         <v>63</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E145" s="2" t="n">
         <v>0</v>
@@ -3655,7 +3652,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3948,7 +3945,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4013,7 +4010,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4197,7 +4194,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
@@ -4230,7 +4227,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.71"/>
@@ -4271,10 +4268,10 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
@@ -5528,7 +5525,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5888,11 +5885,11 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.53"/>
@@ -5907,7 +5904,7 @@
         <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6044,7 +6041,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>261.322247378328</v>
@@ -6052,7 +6049,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>24888.0190416619</v>
@@ -6060,7 +6057,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>13328.4113960832</v>
@@ -6068,7 +6065,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>58.4479914299166</v>
@@ -6076,7 +6073,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>-1724.34876438959</v>

</xml_diff>